<commit_message>
Requirements, Architectures, Coding ReviewReport TODO: - Sonar ReviewReport Sheet - Implement Requirements, Architectures and Coding changes (Mihai)
</commit_message>
<xml_diff>
--- a/Lab01/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Lab01/CheckLists/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laptop\e\VVSS\CamiVVSS_ro2024-2025\Labs\Lab01\CheckListsAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dominic\Domi\Anul 3 Sem 2\VVSS\VVSS-Lab\Lab01\CheckLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C988F33-E974-4516-BC95-27D0B68ECC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CC4242-EF46-4775-9D8C-615CCA21D6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -74,12 +74,6 @@
     <t>Popescu Ionel</t>
   </si>
   <si>
-    <t>Georgescu Anca</t>
-  </si>
-  <si>
-    <t>Firicescu George</t>
-  </si>
-  <si>
     <t>Requirements Document</t>
   </si>
   <si>
@@ -135,6 +129,177 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>Alexandrescu Stefan</t>
+  </si>
+  <si>
+    <t>Bacs Dominic</t>
+  </si>
+  <si>
+    <t>Andrei-Nicoara Sabina Eleny</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Parțial adevărat. Deși enunțul oferă o descriere generală a funcționalităților, lipsesc detalii esențiale, cum ar fi fluxul exact al comenzilor sau interacțiunea dintre utilizatori și sistem.</t>
+  </si>
+  <si>
+    <t>Da. Nu este clar cum se gestionează meniul din fișier text (cum se actualizează sau cum se încarcă inițial). De asemenea, nu este specificat cum sunt distribuite comenzile între mese sau dacă există un sistem de prioritizare.</t>
+  </si>
+  <si>
+    <t>rand 5</t>
+  </si>
+  <si>
+    <t>pag 1</t>
+  </si>
+  <si>
+    <t>rand 3</t>
+  </si>
+  <si>
+    <t>Nu, nimic nu este precizat despre inițializare.</t>
+  </si>
+  <si>
+    <t>rand 14</t>
+  </si>
+  <si>
+    <t>Nu este limpede descris modul in care se afișează totalul încasărilor.</t>
+  </si>
+  <si>
+    <t>randurile 3-8</t>
+  </si>
+  <si>
+    <t>Din păcate, nu este precizat concis dacă soluția software prezintă un tab pentru fiecare utilizator (chelner, bucătar).</t>
+  </si>
+  <si>
+    <t>randurile 1-4</t>
+  </si>
+  <si>
+    <t>Într-adevăr, nu este menționat într-un mod adecvat mediul și interfața pe care va rula această aplicație.</t>
+  </si>
+  <si>
+    <t>0.67 hours</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>PizzaService</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>Georgescu C</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>Diagrama de clase indică o arhitectură clar structurată.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este evidențiată un sistem de clase partiționat corect, cu dependențe clare. </t>
+  </si>
+  <si>
+    <t>Nu există o modalitate de gestionare a erorilor robustă în arhitectură.</t>
+  </si>
+  <si>
+    <t>Doar PaymentRepo ar trebui să creeze instanțe de Payment, nu și PizzaService.</t>
+  </si>
+  <si>
+    <t>PizzaService ar putea fi redenumit într-un mod mai sugestiv, i.e. RestuarantService.</t>
+  </si>
+  <si>
+    <t>Se observă urmarea structurii șabloanelor de proiectare Repository și Model-View-Controller.</t>
+  </si>
+  <si>
+    <t>PizzaService, PaymentRepo</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>PaymentRepository, linia 52</t>
+  </si>
+  <si>
+    <t>La adăugarea unei plăți noi, se rescrie în fișier tot istoricul plăților, în loc ca ultima plată adăugată să fie atașată în fișier.</t>
+  </si>
+  <si>
+    <t>PaymentAlert, liniile 52-56</t>
+  </si>
+  <si>
+    <t>Ulimele două ramuri de else if, respectiv else, ar putea consta într-un singur else cu același corp de execuție.</t>
+  </si>
+  <si>
+    <t>KitchenGUIController, liniile 28-40</t>
+  </si>
+  <si>
+    <t>Nu există nicio condiție de oprire.</t>
+  </si>
+  <si>
+    <t>MenuRepository, linia 11</t>
+  </si>
+  <si>
+    <t>Citirea datelor depinde de calea fișierului și execuția proiectului.</t>
+  </si>
+  <si>
+    <t>Nu.</t>
+  </si>
+  <si>
+    <t>OrdersGUI, linia 20</t>
+  </si>
+  <si>
+    <t>PizzaService este declarat ca field al clasei, dar nu este folosit.</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>filename ar trebui să fie final</t>
   </si>
 </sst>
 </file>
@@ -326,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +521,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -398,7 +564,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,6 +586,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1929816</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>37345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2116802</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>170961</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B48DE37-C0B6-BC73-1609-584971CE5660}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5686085" y="789576"/>
+          <a:ext cx="186986" cy="133616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -708,18 +946,19 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="E1" zoomScale="126" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.90625" style="6"/>
     <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.90625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="21" style="6" customWidth="1"/>
+    <col min="9" max="9" width="24.54296875" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
     <col min="11" max="16384" width="8.90625" style="6"/>
   </cols>
@@ -729,76 +968,92 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="24"/>
+      <c r="D4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="26"/>
+      <c r="D5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="37">
+        <v>45720</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -814,65 +1069,100 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
@@ -962,7 +1252,9 @@
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -985,8 +1277,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="D1" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,76 +1297,92 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="D4" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="D5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="37">
+        <v>45720</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1090,58 +1398,86 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
@@ -1247,7 +1583,9 @@
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1260,6 +1598,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1270,8 +1609,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="B1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1279,7 +1618,7 @@
     <col min="1" max="1" width="8.90625" style="6"/>
     <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.90625" style="6"/>
     <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
@@ -1291,76 +1630,92 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="37">
+        <v>45720</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1376,67 +1731,107 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
@@ -1592,8 +1987,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1614,42 +2009,42 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="H1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+        <v>23</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1658,10 +2053,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1671,8 +2066,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1680,16 +2075,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1902,15 +2297,15 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="C32" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F35" s="35"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Solved a few SonarCube warnings - wrote selected warnings in the Excel file - fixed code
</commit_message>
<xml_diff>
--- a/Lab01/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Lab01/CheckLists/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dominic\Domi\Anul 3 Sem 2\VVSS\VVSS-Lab\Lab01\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Documents\Github\VVSS-Lab\Lab01\CheckLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CC4242-EF46-4775-9D8C-615CCA21D6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DD5EA6-7604-4FC4-93BA-9AF76BDB066F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
-  </si>
-  <si>
     <t>Alexandrescu Stefan</t>
   </si>
   <si>
@@ -300,19 +297,145 @@
   </si>
   <si>
     <t>filename ar trebui să fie final</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java, linia 53</t>
+  </si>
+  <si>
+    <t>Instance methods should not write to "static" fields</t>
+  </si>
+  <si>
+    <t>public void setTotalAmount(double totalAmount) {
+        this.totalAmount = totalAmount;
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public static void setTotalAmount(double totalAmount) {
+        OrdersGUIController.totalAmount = totalAmount;
+    }</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java, linia 65</t>
+  </si>
+  <si>
+    <t>Methods should not be empty</t>
+  </si>
+  <si>
+    <t>public OrdersGUIController(){ }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public OrdersGUIController(){
+        // This constructor is used by FXMLLoader
+    }</t>
+  </si>
+  <si>
+    <t>MenuRepository.java, linia 23</t>
+  </si>
+  <si>
+    <t>Resources should be closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BufferedReader br = null;
+        try {
+            br = new BufferedReader(new FileReader(file));
+            String line = null;
+            while((line=br.readLine())!=null){
+                MenuDataModel menuItem=getMenuItem(line);
+                listMenu.add(menuItem);
+            }
+            br.close();
+        } catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        try(BufferedReader br = new BufferedReader(new FileReader(file))) {
+            String line = null;
+            while((line=br.readLine())!=null){
+                MenuDataModel menuItem=getMenuItem(line);
+                listMenu.add(menuItem);
+            }
+            br.close();
+        } catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>PaymentType.java, linia 4</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t>public enum PaymentType {
+    Cash, Card
+}</t>
+  </si>
+  <si>
+    <t>public enum PaymentType {
+    CASH, CARD
+}
+- am modificat fișierul payments.txt a.î. numele tipurilor de plată să fie cu litere mari, pentru a corespunde cu enum-ul</t>
+  </si>
+  <si>
+    <t>PaymentAlert.java, linia 19, 22, …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    @Override
+    public void cardPayment() {
+        System.out.println("--------------------------");
+        System.out.println("Paying by card...");
+        System.out.println("Please insert your card!");
+        System.out.println("--------------------------");
+    }</t>
+  </si>
+  <si>
+    <t>String literals should not be duplicated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private static final String LINE = "--------------------------";    @Override
+    public void cardPayment() {
+        System.out.println(LINE);
+        System.out.println("Paying by card...");
+        System.out.println("Please insert your card!");
+        System.out.println(LINE);
+    }</t>
+  </si>
+  <si>
+    <t>SonarCube</t>
+  </si>
+  <si>
+    <t>Alexandrescu Stefan, Andrei-Nicoara Sabina-Eleny</t>
+  </si>
+  <si>
+    <t>04.03.2025</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -491,86 +614,111 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,19 +1116,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -993,8 +1141,8 @@
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>31</v>
+      <c r="I3" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1004,15 +1152,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>33</v>
+      <c r="I4" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1022,15 +1170,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="27"/>
+      <c r="D5" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>32</v>
+      <c r="I5" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="J5" s="3">
         <v>231</v>
@@ -1041,19 +1189,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="24">
         <v>45720</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1069,18 +1217,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
@@ -1089,13 +1237,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1104,13 +1252,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1119,13 +1267,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1134,13 +1282,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1149,13 +1297,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1253,7 +1401,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1425,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D15" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1297,19 +1445,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -1322,8 +1470,8 @@
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="40" t="s">
-        <v>31</v>
+      <c r="I3" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1333,15 +1481,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="40" t="s">
-        <v>33</v>
+      <c r="I4" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1351,15 +1499,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="30"/>
+      <c r="D5" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="40" t="s">
-        <v>32</v>
+      <c r="I5" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="J5" s="3">
         <v>231</v>
@@ -1370,19 +1518,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="24">
         <v>45720</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1403,11 +1551,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1416,11 +1564,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1429,11 +1577,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1442,11 +1590,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1455,13 +1603,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1470,13 +1618,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1584,7 +1732,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1609,8 +1757,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+    <sheetView topLeftCell="B18" zoomScale="103" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1630,19 +1778,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -1655,8 +1803,8 @@
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="40" t="s">
-        <v>31</v>
+      <c r="I3" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="J3" s="17">
         <v>231</v>
@@ -1666,15 +1814,15 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="40" t="s">
-        <v>33</v>
+      <c r="I4" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="J4" s="3">
         <v>231</v>
@@ -1684,15 +1832,15 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="40" t="s">
-        <v>32</v>
+      <c r="I5" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="J5" s="3">
         <v>231</v>
@@ -1703,19 +1851,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="24">
         <v>45720</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1736,13 +1884,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1751,13 +1899,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1766,13 +1914,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1781,13 +1929,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1796,11 +1944,11 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1809,13 +1957,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1824,13 +1972,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
@@ -1964,7 +2112,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1987,18 +2137,18 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.90625" style="6"/>
     <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="36.81640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="42.1796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="49.6328125" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.90625" style="6"/>
     <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.90625" style="6"/>
@@ -2009,19 +2159,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -2034,40 +2184,58 @@
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="3">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -2087,221 +2255,261 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
+    <row r="10" spans="1:10" s="43" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="46">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="3">
+      <c r="C10" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="43" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="46">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
+      <c r="C11" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="43" customFormat="1" ht="232" x14ac:dyDescent="0.35">
+      <c r="B12" s="46">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
+      <c r="C12" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="43" customFormat="1" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
+      <c r="C13" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="43" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="B14" s="46">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
+      <c r="C14" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="46">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="3">
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+    </row>
+    <row r="16" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="46">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="3">
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+    </row>
+    <row r="17" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="46">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="3">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+    </row>
+    <row r="18" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="46">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="3">
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="46">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="3">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="46">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="3">
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+    </row>
+    <row r="21" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="46">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="3">
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="46">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="3">
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+    </row>
+    <row r="23" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="46">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="3">
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+    </row>
+    <row r="24" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="3">
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+    </row>
+    <row r="25" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="46">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="3">
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+    </row>
+    <row r="26" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="40">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="3">
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+    </row>
+    <row r="27" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="40">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="3">
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+    </row>
+    <row r="28" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="40">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="3">
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+    </row>
+    <row r="29" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="40">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="3">
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+    </row>
+    <row r="30" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="40">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="C32" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Improved requirements, architecture, and added corresponding code to reflect the observations.
</commit_message>
<xml_diff>
--- a/Lab01/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Lab01/CheckLists/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Documents\Github\VVSS-Lab\Lab01\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Documents\GitHub\VVSS-Lab\Lab01\CheckLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DD5EA6-7604-4FC4-93BA-9AF76BDB066F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BBBA0-3F0B-4DF4-A704-8383E38A4C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="3315" windowWidth="26520" windowHeight="16170" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -170,15 +170,9 @@
     <t>rand 3</t>
   </si>
   <si>
-    <t>Nu, nimic nu este precizat despre inițializare.</t>
-  </si>
-  <si>
     <t>rand 14</t>
   </si>
   <si>
-    <t>Nu este limpede descris modul in care se afișează totalul încasărilor.</t>
-  </si>
-  <si>
     <t>randurile 3-8</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>A01</t>
   </si>
   <si>
-    <t>A09</t>
-  </si>
-  <si>
     <t>Georgescu C</t>
   </si>
   <si>
@@ -221,24 +212,12 @@
     <t>Diagrama de clase indică o arhitectură clar structurată.</t>
   </si>
   <si>
-    <t xml:space="preserve">Este evidențiată un sistem de clase partiționat corect, cu dependențe clare. </t>
-  </si>
-  <si>
     <t>Nu există o modalitate de gestionare a erorilor robustă în arhitectură.</t>
   </si>
   <si>
-    <t>Doar PaymentRepo ar trebui să creeze instanțe de Payment, nu și PizzaService.</t>
-  </si>
-  <si>
     <t>PizzaService ar putea fi redenumit într-un mod mai sugestiv, i.e. RestuarantService.</t>
   </si>
   <si>
-    <t>Se observă urmarea structurii șabloanelor de proiectare Repository și Model-View-Controller.</t>
-  </si>
-  <si>
-    <t>PizzaService, PaymentRepo</t>
-  </si>
-  <si>
     <t>0.6</t>
   </si>
   <si>
@@ -254,9 +233,6 @@
     <t>C05</t>
   </si>
   <si>
-    <t>C06</t>
-  </si>
-  <si>
     <t>C09</t>
   </si>
   <si>
@@ -279,9 +255,6 @@
   </si>
   <si>
     <t>MenuRepository, linia 11</t>
-  </si>
-  <si>
-    <t>Citirea datelor depinde de calea fișierului și execuția proiectului.</t>
   </si>
   <si>
     <t>Nu.</t>
@@ -416,6 +389,30 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours): 0.5</t>
+  </si>
+  <si>
+    <t>Nu, nimic nu este precizat despre inițializarea aplicației.</t>
+  </si>
+  <si>
+    <t>Nu este limpede descris modul in care se afișează totalul încasărilor, respectiv perioada din care se calculează încasările.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este evidențiat un sistem de clase partiționat corect, cu dependențe clare. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se observă urmarea structurii șabloanelor de proiectare Repository și Model-View-Controller. De asemenea, în KitchenGUIController, ar putea fi utilizate mecanisme de Observer Pattern, care lipsesc în acest moment. </t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Există un element ce aparține de layerul de Model din UI (i.e. MenuDataModel, având proprietăți specifice JavaFX), ce n-ar trebui utilizat de către clase din layerele de Business sau Repository, așa cum este în acest moment.</t>
+  </si>
+  <si>
+    <t>Tot proiectul/ KitchenGUIController</t>
+  </si>
+  <si>
+    <t>PizzaService, MenuRepository, MenuDataModel</t>
   </si>
 </sst>
 </file>
@@ -647,6 +644,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -691,33 +715,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,13 +738,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1929816</xdr:colOff>
+      <xdr:colOff>1831281</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>37345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2116802</xdr:colOff>
+      <xdr:colOff>2018267</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>170961</xdr:rowOff>
     </xdr:to>
@@ -779,7 +776,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5686085" y="789576"/>
+          <a:off x="5411367" y="805914"/>
           <a:ext cx="186986" cy="133616"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1094,41 +1091,41 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="126" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J5"/>
+    <sheetView zoomScale="126" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.90625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="24.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -1137,7 +1134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
@@ -1148,14 +1145,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="37"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
@@ -1166,14 +1163,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="39"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1184,26 +1181,26 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="33">
         <v>45720</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E7" s="34"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1217,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1231,7 +1228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1246,7 +1243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1258,10 +1255,10 @@
         <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1270,13 +1267,13 @@
         <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1285,13 +1282,13 @@
         <v>37</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1300,13 +1297,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1314,7 +1311,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1323,7 +1320,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1332,7 +1329,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1341,7 +1338,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1350,7 +1347,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1359,7 +1356,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1368,7 +1365,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1377,7 +1374,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1386,7 +1383,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1395,13 +1392,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1425,39 +1422,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="D15" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -1466,7 +1463,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
@@ -1477,14 +1474,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="40"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
@@ -1495,14 +1492,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="33"/>
+      <c r="D5" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="42"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1513,26 +1510,26 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="33">
         <v>45720</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E7" s="34"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1546,88 +1543,90 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>106</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1636,7 +1635,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1645,7 +1644,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1654,7 +1653,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1663,7 +1662,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1672,7 +1671,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1681,7 +1680,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1690,7 +1689,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1699,7 +1698,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1708,7 +1707,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1717,7 +1716,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1726,13 +1725,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1755,42 +1754,42 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="B1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="B11" sqref="A11:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -1799,7 +1798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
@@ -1810,14 +1809,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="43"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
@@ -1828,14 +1827,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="45"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1846,26 +1845,26 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="33">
         <v>45720</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E7" s="34"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1879,109 +1878,103 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <f t="shared" ref="B12:B29" si="0">B11+1</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
-        <f t="shared" ref="B12:B30" si="0">B11+1</f>
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1990,43 +1983,43 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2035,7 +2028,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2044,7 +2037,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2053,34 +2046,34 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2089,7 +2082,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2098,21 +2091,12 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C32" s="11" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="1">
+      <c r="D31" s="12"/>
+      <c r="E31" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -2137,41 +2121,41 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="C6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="36.81640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="42.1796875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="49.6328125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>28</v>
@@ -2180,7 +2164,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
@@ -2191,14 +2175,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="34"/>
+      <c r="D4" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="43"/>
       <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
@@ -2209,14 +2193,14 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="25"/>
+      <c r="D5" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
@@ -2227,18 +2211,18 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="25"/>
+      <c r="D6" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="34"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2255,264 +2239,264 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="43" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="46">
+    <row r="10" spans="1:10" s="28" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="31">
         <v>1</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="43" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="46">
+      <c r="C10" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="31">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="43" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="B12" s="46">
+      <c r="C11" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="28" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+      <c r="B12" s="31">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="28" customFormat="1" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="28" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="B14" s="31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="45" t="s">
+      <c r="F14" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="43" customFormat="1" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="46">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="45" t="s">
+    </row>
+    <row r="15" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="31">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+    </row>
+    <row r="16" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="31">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="31">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="31">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="31">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="31">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="31">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+    </row>
+    <row r="24" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="31">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="2:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="31">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+    </row>
+    <row r="26" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+    </row>
+    <row r="29" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+    </row>
+    <row r="30" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="45" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="43" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="B14" s="46">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="46">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-    </row>
-    <row r="16" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="46">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="46">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-    </row>
-    <row r="18" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="46">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-    </row>
-    <row r="19" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-    </row>
-    <row r="20" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="46">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-    </row>
-    <row r="21" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="46">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="46">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-    </row>
-    <row r="23" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="46">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-    </row>
-    <row r="24" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="46">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-    </row>
-    <row r="25" spans="2:6" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="46">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-    </row>
-    <row r="26" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="40">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-    </row>
-    <row r="27" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="40">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-    </row>
-    <row r="28" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="40">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-    </row>
-    <row r="29" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="40">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-    </row>
-    <row r="30" spans="2:6" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="40">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>